<commit_message>
Alterados os metodos get e set para open e save nas classes DAO
</commit_message>
<xml_diff>
--- a/SorteioGrupos/documentos/ContasBalanco.xlsx
+++ b/SorteioGrupos/documentos/ContasBalanco.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARQUIVOS\SENAI\Planos_Ensino\2020_2_Semestre\ProjetoIntegrador\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARQUIVOS\SENAI\Planos_Ensino\2020_2_Semestre\ProjetoIntegrador1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7513ADEA-D107-4531-8B52-4B011582A607}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8569172-DF9E-4A3E-9D82-09A79B91B39A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A2EFEAD8-89AC-4165-9D5E-89350841DA2B}"/>
+    <workbookView minimized="1" xWindow="735" yWindow="735" windowWidth="14730" windowHeight="9000" activeTab="1" xr2:uid="{A2EFEAD8-89AC-4165-9D5E-89350841DA2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Contas" sheetId="5" r:id="rId1"/>
@@ -556,7 +556,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{640CAE45-5790-46A8-807A-DA04193D1F83}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -814,7 +816,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80841558-75D0-42C2-96BC-AE19C3CE2319}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -853,11 +857,11 @@
         <v>1</v>
       </c>
       <c r="C2" t="str">
-        <f>VLOOKUP(B2,contas,2)</f>
+        <f t="shared" ref="C2:C31" si="0">VLOOKUP(B2,contas,2)</f>
         <v>Débito</v>
       </c>
       <c r="D2" t="str">
-        <f>VLOOKUP(B2,contas,4)</f>
+        <f t="shared" ref="D2:D31" si="1">VLOOKUP(B2,contas,4)</f>
         <v>Pagamento de Aluguél</v>
       </c>
       <c r="E2" s="2">
@@ -879,11 +883,11 @@
         <v>3</v>
       </c>
       <c r="C3" t="str">
-        <f>VLOOKUP(B3,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D3" t="str">
-        <f>VLOOKUP(B3,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Conta de Energia Elétrica</v>
       </c>
       <c r="E3" s="2">
@@ -905,11 +909,11 @@
         <v>7</v>
       </c>
       <c r="C4" t="str">
-        <f>VLOOKUP(B4,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D4" t="str">
-        <f>VLOOKUP(B4,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Multa</v>
       </c>
       <c r="E4" s="2">
@@ -931,11 +935,11 @@
         <v>12</v>
       </c>
       <c r="C5" t="str">
-        <f>VLOOKUP(B5,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D5" t="str">
-        <f>VLOOKUP(B5,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Fatura a Fornecedor</v>
       </c>
       <c r="E5" s="2">
@@ -950,11 +954,11 @@
         <v>15</v>
       </c>
       <c r="C6" t="str">
-        <f>VLOOKUP(B6,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D6" t="str">
-        <f>VLOOKUP(B6,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Recebimento de Juros por atraso em parcela</v>
       </c>
       <c r="E6" s="2">
@@ -969,11 +973,11 @@
         <v>4</v>
       </c>
       <c r="C7" t="str">
-        <f>VLOOKUP(B7,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D7" t="str">
-        <f>VLOOKUP(B7,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Conta de Telefone</v>
       </c>
       <c r="E7" s="2">
@@ -988,11 +992,11 @@
         <v>6</v>
       </c>
       <c r="C8" t="str">
-        <f>VLOOKUP(B8,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D8" t="str">
-        <f>VLOOKUP(B8,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagemento de Salário</v>
       </c>
       <c r="E8" s="2">
@@ -1007,11 +1011,11 @@
         <v>7</v>
       </c>
       <c r="C9" t="str">
-        <f>VLOOKUP(B9,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D9" t="str">
-        <f>VLOOKUP(B9,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Multa</v>
       </c>
       <c r="E9" s="2">
@@ -1026,11 +1030,11 @@
         <v>9</v>
       </c>
       <c r="C10" t="str">
-        <f>VLOOKUP(B10,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D10" t="str">
-        <f>VLOOKUP(B10,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Aporte de Investimento em Renda Fixa</v>
       </c>
       <c r="E10" s="2">
@@ -1045,11 +1049,11 @@
         <v>8</v>
       </c>
       <c r="C11" t="str">
-        <f>VLOOKUP(B11,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D11" t="str">
-        <f>VLOOKUP(B11,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Aporte de Investimento em Ações</v>
       </c>
       <c r="E11" s="2">
@@ -1064,11 +1068,11 @@
         <v>5</v>
       </c>
       <c r="C12" t="str">
-        <f>VLOOKUP(B12,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D12" t="str">
-        <f>VLOOKUP(B12,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Conta de Internet</v>
       </c>
       <c r="E12" s="2">
@@ -1083,11 +1087,11 @@
         <v>11</v>
       </c>
       <c r="C13" t="str">
-        <f>VLOOKUP(B13,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D13" t="str">
-        <f>VLOOKUP(B13,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Compra de Equipamentos</v>
       </c>
       <c r="E13" s="2">
@@ -1102,11 +1106,11 @@
         <v>12</v>
       </c>
       <c r="C14" t="str">
-        <f>VLOOKUP(B14,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D14" t="str">
-        <f>VLOOKUP(B14,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Fatura a Fornecedor</v>
       </c>
       <c r="E14" s="2">
@@ -1121,11 +1125,11 @@
         <v>13</v>
       </c>
       <c r="C15" t="str">
-        <f>VLOOKUP(B15,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D15" t="str">
-        <f>VLOOKUP(B15,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Venda diréta à vista</v>
       </c>
       <c r="E15" s="2">
@@ -1140,11 +1144,11 @@
         <v>14</v>
       </c>
       <c r="C16" t="str">
-        <f>VLOOKUP(B16,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D16" t="str">
-        <f>VLOOKUP(B16,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Recebimento de Parcela de Venda à praso</v>
       </c>
       <c r="E16" s="2">
@@ -1159,11 +1163,11 @@
         <v>15</v>
       </c>
       <c r="C17" t="str">
-        <f>VLOOKUP(B17,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D17" t="str">
-        <f>VLOOKUP(B17,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Recebimento de Juros por atraso em parcela</v>
       </c>
       <c r="E17" s="2">
@@ -1178,11 +1182,11 @@
         <v>12</v>
       </c>
       <c r="C18" t="str">
-        <f>VLOOKUP(B18,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D18" t="str">
-        <f>VLOOKUP(B18,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Fatura a Fornecedor</v>
       </c>
       <c r="E18" s="2">
@@ -1197,11 +1201,11 @@
         <v>2</v>
       </c>
       <c r="C19" t="str">
-        <f>VLOOKUP(B19,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D19" t="str">
-        <f>VLOOKUP(B19,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Conta de Água</v>
       </c>
       <c r="E19" s="2">
@@ -1216,11 +1220,11 @@
         <v>6</v>
       </c>
       <c r="C20" t="str">
-        <f>VLOOKUP(B20,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D20" t="str">
-        <f>VLOOKUP(B20,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagemento de Salário</v>
       </c>
       <c r="E20" s="2">
@@ -1235,11 +1239,11 @@
         <v>16</v>
       </c>
       <c r="C21" t="str">
-        <f>VLOOKUP(B21,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D21" t="str">
-        <f>VLOOKUP(B21,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Recebimento de Rendimento em investimento</v>
       </c>
       <c r="E21" s="2">
@@ -1254,11 +1258,11 @@
         <v>13</v>
       </c>
       <c r="C22" t="str">
-        <f>VLOOKUP(B22,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D22" t="str">
-        <f>VLOOKUP(B22,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Venda diréta à vista</v>
       </c>
       <c r="E22" s="2">
@@ -1273,11 +1277,11 @@
         <v>12</v>
       </c>
       <c r="C23" t="str">
-        <f>VLOOKUP(B23,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D23" t="str">
-        <f>VLOOKUP(B23,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Fatura a Fornecedor</v>
       </c>
       <c r="E23" s="2">
@@ -1292,11 +1296,11 @@
         <v>12</v>
       </c>
       <c r="C24" t="str">
-        <f>VLOOKUP(B24,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D24" t="str">
-        <f>VLOOKUP(B24,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Fatura a Fornecedor</v>
       </c>
       <c r="E24" s="2">
@@ -1311,11 +1315,11 @@
         <v>13</v>
       </c>
       <c r="C25" t="str">
-        <f>VLOOKUP(B25,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D25" t="str">
-        <f>VLOOKUP(B25,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Venda diréta à vista</v>
       </c>
       <c r="E25" s="2">
@@ -1330,11 +1334,11 @@
         <v>13</v>
       </c>
       <c r="C26" t="str">
-        <f>VLOOKUP(B26,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D26" t="str">
-        <f>VLOOKUP(B26,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Venda diréta à vista</v>
       </c>
       <c r="E26" s="2">
@@ -1349,11 +1353,11 @@
         <v>12</v>
       </c>
       <c r="C27" t="str">
-        <f>VLOOKUP(B27,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D27" t="str">
-        <f>VLOOKUP(B27,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Fatura a Fornecedor</v>
       </c>
       <c r="E27" s="2">
@@ -1368,11 +1372,11 @@
         <v>13</v>
       </c>
       <c r="C28" t="str">
-        <f>VLOOKUP(B28,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D28" t="str">
-        <f>VLOOKUP(B28,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Venda diréta à vista</v>
       </c>
       <c r="E28" s="2">
@@ -1387,11 +1391,11 @@
         <v>14</v>
       </c>
       <c r="C29" t="str">
-        <f>VLOOKUP(B29,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D29" t="str">
-        <f>VLOOKUP(B29,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Recebimento de Parcela de Venda à praso</v>
       </c>
       <c r="E29" s="2">
@@ -1406,11 +1410,11 @@
         <v>14</v>
       </c>
       <c r="C30" t="str">
-        <f>VLOOKUP(B30,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D30" t="str">
-        <f>VLOOKUP(B30,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Recebimento de Parcela de Venda à praso</v>
       </c>
       <c r="E30" s="2">
@@ -1425,11 +1429,11 @@
         <v>14</v>
       </c>
       <c r="C31" t="str">
-        <f>VLOOKUP(B31,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D31" t="str">
-        <f>VLOOKUP(B31,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Recebimento de Parcela de Venda à praso</v>
       </c>
       <c r="E31" s="2">
@@ -1465,7 +1469,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F33462E-AC81-4275-9710-E3B0C49A647B}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1504,11 +1510,11 @@
         <v>1</v>
       </c>
       <c r="C2" t="str">
-        <f>VLOOKUP(B2,contas,2)</f>
+        <f t="shared" ref="C2:C28" si="0">VLOOKUP(B2,contas,2)</f>
         <v>Débito</v>
       </c>
       <c r="D2" t="str">
-        <f>VLOOKUP(B2,contas,4)</f>
+        <f t="shared" ref="D2:D28" si="1">VLOOKUP(B2,contas,4)</f>
         <v>Pagamento de Aluguél</v>
       </c>
       <c r="E2" s="2">
@@ -1530,11 +1536,11 @@
         <v>3</v>
       </c>
       <c r="C3" t="str">
-        <f>VLOOKUP(B3,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D3" t="str">
-        <f>VLOOKUP(B3,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Conta de Energia Elétrica</v>
       </c>
       <c r="E3" s="2">
@@ -1556,11 +1562,11 @@
         <v>7</v>
       </c>
       <c r="C4" t="str">
-        <f>VLOOKUP(B4,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D4" t="str">
-        <f>VLOOKUP(B4,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Multa</v>
       </c>
       <c r="E4" s="2">
@@ -1582,11 +1588,11 @@
         <v>12</v>
       </c>
       <c r="C5" t="str">
-        <f>VLOOKUP(B5,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D5" t="str">
-        <f>VLOOKUP(B5,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Fatura a Fornecedor</v>
       </c>
       <c r="E5" s="2">
@@ -1601,11 +1607,11 @@
         <v>15</v>
       </c>
       <c r="C6" t="str">
-        <f>VLOOKUP(B6,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D6" t="str">
-        <f>VLOOKUP(B6,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Recebimento de Juros por atraso em parcela</v>
       </c>
       <c r="E6" s="2">
@@ -1620,11 +1626,11 @@
         <v>4</v>
       </c>
       <c r="C7" t="str">
-        <f>VLOOKUP(B7,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D7" t="str">
-        <f>VLOOKUP(B7,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Conta de Telefone</v>
       </c>
       <c r="E7" s="2">
@@ -1639,11 +1645,11 @@
         <v>6</v>
       </c>
       <c r="C8" t="str">
-        <f>VLOOKUP(B8,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D8" t="str">
-        <f>VLOOKUP(B8,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagemento de Salário</v>
       </c>
       <c r="E8" s="2">
@@ -1658,11 +1664,11 @@
         <v>7</v>
       </c>
       <c r="C9" t="str">
-        <f>VLOOKUP(B9,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D9" t="str">
-        <f>VLOOKUP(B9,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Multa</v>
       </c>
       <c r="E9" s="2">
@@ -1677,11 +1683,11 @@
         <v>9</v>
       </c>
       <c r="C10" t="str">
-        <f>VLOOKUP(B10,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D10" t="str">
-        <f>VLOOKUP(B10,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Aporte de Investimento em Renda Fixa</v>
       </c>
       <c r="E10" s="2">
@@ -1696,11 +1702,11 @@
         <v>8</v>
       </c>
       <c r="C11" t="str">
-        <f>VLOOKUP(B11,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D11" t="str">
-        <f>VLOOKUP(B11,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Aporte de Investimento em Ações</v>
       </c>
       <c r="E11" s="2">
@@ -1715,11 +1721,11 @@
         <v>5</v>
       </c>
       <c r="C12" t="str">
-        <f>VLOOKUP(B12,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D12" t="str">
-        <f>VLOOKUP(B12,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Conta de Internet</v>
       </c>
       <c r="E12" s="2">
@@ -1734,11 +1740,11 @@
         <v>11</v>
       </c>
       <c r="C13" t="str">
-        <f>VLOOKUP(B13,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D13" t="str">
-        <f>VLOOKUP(B13,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Compra de Equipamentos</v>
       </c>
       <c r="E13" s="2">
@@ -1753,11 +1759,11 @@
         <v>12</v>
       </c>
       <c r="C14" t="str">
-        <f>VLOOKUP(B14,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D14" t="str">
-        <f>VLOOKUP(B14,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Fatura a Fornecedor</v>
       </c>
       <c r="E14" s="2">
@@ -1772,11 +1778,11 @@
         <v>14</v>
       </c>
       <c r="C15" t="str">
-        <f>VLOOKUP(B15,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D15" t="str">
-        <f>VLOOKUP(B15,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Recebimento de Parcela de Venda à praso</v>
       </c>
       <c r="E15" s="2">
@@ -1791,11 +1797,11 @@
         <v>15</v>
       </c>
       <c r="C16" t="str">
-        <f>VLOOKUP(B16,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D16" t="str">
-        <f>VLOOKUP(B16,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Recebimento de Juros por atraso em parcela</v>
       </c>
       <c r="E16" s="2">
@@ -1810,11 +1816,11 @@
         <v>12</v>
       </c>
       <c r="C17" t="str">
-        <f>VLOOKUP(B17,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D17" t="str">
-        <f>VLOOKUP(B17,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Fatura a Fornecedor</v>
       </c>
       <c r="E17" s="2">
@@ -1829,11 +1835,11 @@
         <v>2</v>
       </c>
       <c r="C18" t="str">
-        <f>VLOOKUP(B18,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D18" t="str">
-        <f>VLOOKUP(B18,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Conta de Água</v>
       </c>
       <c r="E18" s="2">
@@ -1848,11 +1854,11 @@
         <v>6</v>
       </c>
       <c r="C19" t="str">
-        <f>VLOOKUP(B19,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D19" t="str">
-        <f>VLOOKUP(B19,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagemento de Salário</v>
       </c>
       <c r="E19" s="2">
@@ -1867,11 +1873,11 @@
         <v>16</v>
       </c>
       <c r="C20" t="str">
-        <f>VLOOKUP(B20,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D20" t="str">
-        <f>VLOOKUP(B20,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Recebimento de Rendimento em investimento</v>
       </c>
       <c r="E20" s="2">
@@ -1886,11 +1892,11 @@
         <v>12</v>
       </c>
       <c r="C21" t="str">
-        <f>VLOOKUP(B21,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D21" t="str">
-        <f>VLOOKUP(B21,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Fatura a Fornecedor</v>
       </c>
       <c r="E21" s="2">
@@ -1905,11 +1911,11 @@
         <v>12</v>
       </c>
       <c r="C22" t="str">
-        <f>VLOOKUP(B22,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D22" t="str">
-        <f>VLOOKUP(B22,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Fatura a Fornecedor</v>
       </c>
       <c r="E22" s="2">
@@ -1924,11 +1930,11 @@
         <v>13</v>
       </c>
       <c r="C23" t="str">
-        <f>VLOOKUP(B23,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D23" t="str">
-        <f>VLOOKUP(B23,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Venda diréta à vista</v>
       </c>
       <c r="E23" s="2">
@@ -1943,11 +1949,11 @@
         <v>13</v>
       </c>
       <c r="C24" t="str">
-        <f>VLOOKUP(B24,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D24" t="str">
-        <f>VLOOKUP(B24,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Venda diréta à vista</v>
       </c>
       <c r="E24" s="2">
@@ -1962,11 +1968,11 @@
         <v>12</v>
       </c>
       <c r="C25" t="str">
-        <f>VLOOKUP(B25,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D25" t="str">
-        <f>VLOOKUP(B25,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Fatura a Fornecedor</v>
       </c>
       <c r="E25" s="2">
@@ -1981,11 +1987,11 @@
         <v>13</v>
       </c>
       <c r="C26" t="str">
-        <f>VLOOKUP(B26,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D26" t="str">
-        <f>VLOOKUP(B26,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Venda diréta à vista</v>
       </c>
       <c r="E26" s="2">
@@ -2000,11 +2006,11 @@
         <v>14</v>
       </c>
       <c r="C27" t="str">
-        <f>VLOOKUP(B27,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D27" t="str">
-        <f>VLOOKUP(B27,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Recebimento de Parcela de Venda à praso</v>
       </c>
       <c r="E27" s="2">
@@ -2019,11 +2025,11 @@
         <v>14</v>
       </c>
       <c r="C28" t="str">
-        <f>VLOOKUP(B28,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D28" t="str">
-        <f>VLOOKUP(B28,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Recebimento de Parcela de Venda à praso</v>
       </c>
       <c r="E28" s="2">
@@ -2098,11 +2104,11 @@
         <v>13</v>
       </c>
       <c r="C2" t="str">
-        <f>VLOOKUP(B2,contas,2)</f>
+        <f t="shared" ref="C2:C26" si="0">VLOOKUP(B2,contas,2)</f>
         <v>Crédito</v>
       </c>
       <c r="D2" t="str">
-        <f>VLOOKUP(B2,contas,4)</f>
+        <f t="shared" ref="D2:D26" si="1">VLOOKUP(B2,contas,4)</f>
         <v>Venda diréta à vista</v>
       </c>
       <c r="E2" s="2">
@@ -2124,11 +2130,11 @@
         <v>12</v>
       </c>
       <c r="C3" t="str">
-        <f>VLOOKUP(B3,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D3" t="str">
-        <f>VLOOKUP(B3,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Fatura a Fornecedor</v>
       </c>
       <c r="E3" s="2">
@@ -2150,11 +2156,11 @@
         <v>13</v>
       </c>
       <c r="C4" t="str">
-        <f>VLOOKUP(B4,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D4" t="str">
-        <f>VLOOKUP(B4,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Venda diréta à vista</v>
       </c>
       <c r="E4" s="2">
@@ -2176,11 +2182,11 @@
         <v>15</v>
       </c>
       <c r="C5" t="str">
-        <f>VLOOKUP(B5,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D5" t="str">
-        <f>VLOOKUP(B5,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Recebimento de Juros por atraso em parcela</v>
       </c>
       <c r="E5" s="2">
@@ -2195,11 +2201,11 @@
         <v>4</v>
       </c>
       <c r="C6" t="str">
-        <f>VLOOKUP(B6,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D6" t="str">
-        <f>VLOOKUP(B6,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Conta de Telefone</v>
       </c>
       <c r="E6" s="2">
@@ -2214,11 +2220,11 @@
         <v>12</v>
       </c>
       <c r="C7" t="str">
-        <f>VLOOKUP(B7,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D7" t="str">
-        <f>VLOOKUP(B7,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Fatura a Fornecedor</v>
       </c>
       <c r="E7" s="2">
@@ -2233,11 +2239,11 @@
         <v>7</v>
       </c>
       <c r="C8" t="str">
-        <f>VLOOKUP(B8,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D8" t="str">
-        <f>VLOOKUP(B8,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Multa</v>
       </c>
       <c r="E8" s="2">
@@ -2252,11 +2258,11 @@
         <v>9</v>
       </c>
       <c r="C9" t="str">
-        <f>VLOOKUP(B9,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D9" t="str">
-        <f>VLOOKUP(B9,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Aporte de Investimento em Renda Fixa</v>
       </c>
       <c r="E9" s="2">
@@ -2271,11 +2277,11 @@
         <v>10</v>
       </c>
       <c r="C10" t="str">
-        <f>VLOOKUP(B10,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D10" t="str">
-        <f>VLOOKUP(B10,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Compra direta de Matéria Prima à vista</v>
       </c>
       <c r="E10" s="2">
@@ -2290,11 +2296,11 @@
         <v>1</v>
       </c>
       <c r="C11" t="str">
-        <f>VLOOKUP(B11,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D11" t="str">
-        <f>VLOOKUP(B11,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Aluguél</v>
       </c>
       <c r="E11" s="2">
@@ -2309,11 +2315,11 @@
         <v>12</v>
       </c>
       <c r="C12" t="str">
-        <f>VLOOKUP(B12,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D12" t="str">
-        <f>VLOOKUP(B12,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Fatura a Fornecedor</v>
       </c>
       <c r="E12" s="2">
@@ -2328,11 +2334,11 @@
         <v>13</v>
       </c>
       <c r="C13" t="str">
-        <f>VLOOKUP(B13,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D13" t="str">
-        <f>VLOOKUP(B13,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Venda diréta à vista</v>
       </c>
       <c r="E13" s="2">
@@ -2347,11 +2353,11 @@
         <v>14</v>
       </c>
       <c r="C14" t="str">
-        <f>VLOOKUP(B14,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D14" t="str">
-        <f>VLOOKUP(B14,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Recebimento de Parcela de Venda à praso</v>
       </c>
       <c r="E14" s="2">
@@ -2366,11 +2372,11 @@
         <v>15</v>
       </c>
       <c r="C15" t="str">
-        <f>VLOOKUP(B15,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D15" t="str">
-        <f>VLOOKUP(B15,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Recebimento de Juros por atraso em parcela</v>
       </c>
       <c r="E15" s="2">
@@ -2385,11 +2391,11 @@
         <v>12</v>
       </c>
       <c r="C16" t="str">
-        <f>VLOOKUP(B16,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D16" t="str">
-        <f>VLOOKUP(B16,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Fatura a Fornecedor</v>
       </c>
       <c r="E16" s="2">
@@ -2404,11 +2410,11 @@
         <v>14</v>
       </c>
       <c r="C17" t="str">
-        <f>VLOOKUP(B17,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D17" t="str">
-        <f>VLOOKUP(B17,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Recebimento de Parcela de Venda à praso</v>
       </c>
       <c r="E17" s="2">
@@ -2423,11 +2429,11 @@
         <v>16</v>
       </c>
       <c r="C18" t="str">
-        <f>VLOOKUP(B18,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D18" t="str">
-        <f>VLOOKUP(B18,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Recebimento de Rendimento em investimento</v>
       </c>
       <c r="E18" s="2">
@@ -2442,11 +2448,11 @@
         <v>13</v>
       </c>
       <c r="C19" t="str">
-        <f>VLOOKUP(B19,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D19" t="str">
-        <f>VLOOKUP(B19,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Venda diréta à vista</v>
       </c>
       <c r="E19" s="2">
@@ -2461,11 +2467,11 @@
         <v>13</v>
       </c>
       <c r="C20" t="str">
-        <f>VLOOKUP(B20,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D20" t="str">
-        <f>VLOOKUP(B20,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Venda diréta à vista</v>
       </c>
       <c r="E20" s="2">
@@ -2480,11 +2486,11 @@
         <v>12</v>
       </c>
       <c r="C21" t="str">
-        <f>VLOOKUP(B21,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D21" t="str">
-        <f>VLOOKUP(B21,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Fatura a Fornecedor</v>
       </c>
       <c r="E21" s="2">
@@ -2499,11 +2505,11 @@
         <v>13</v>
       </c>
       <c r="C22" t="str">
-        <f>VLOOKUP(B22,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D22" t="str">
-        <f>VLOOKUP(B22,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Venda diréta à vista</v>
       </c>
       <c r="E22" s="2">
@@ -2518,11 +2524,11 @@
         <v>12</v>
       </c>
       <c r="C23" t="str">
-        <f>VLOOKUP(B23,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Débito</v>
       </c>
       <c r="D23" t="str">
-        <f>VLOOKUP(B23,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Pagamento de Fatura a Fornecedor</v>
       </c>
       <c r="E23" s="2">
@@ -2537,11 +2543,11 @@
         <v>13</v>
       </c>
       <c r="C24" t="str">
-        <f>VLOOKUP(B24,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D24" t="str">
-        <f>VLOOKUP(B24,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Venda diréta à vista</v>
       </c>
       <c r="E24" s="2">
@@ -2556,11 +2562,11 @@
         <v>14</v>
       </c>
       <c r="C25" t="str">
-        <f>VLOOKUP(B25,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D25" t="str">
-        <f>VLOOKUP(B25,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Recebimento de Parcela de Venda à praso</v>
       </c>
       <c r="E25" s="2">
@@ -2575,11 +2581,11 @@
         <v>13</v>
       </c>
       <c r="C26" t="str">
-        <f>VLOOKUP(B26,contas,2)</f>
+        <f t="shared" si="0"/>
         <v>Crédito</v>
       </c>
       <c r="D26" t="str">
-        <f>VLOOKUP(B26,contas,4)</f>
+        <f t="shared" si="1"/>
         <v>Venda diréta à vista</v>
       </c>
       <c r="E26" s="2">

</xml_diff>